<commit_message>
small corrections after testing the workflow
</commit_message>
<xml_diff>
--- a/EFA results/freq_pers_obl_4.xlsx
+++ b/EFA results/freq_pers_obl_4.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,55 +370,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>item_name</t>
+          <t>X1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>item_text_english</t>
+          <t>X2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>item_name</t>
+          <t>X3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>item_text_english</t>
+          <t>X4</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>X1</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>X2</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>X3</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>X4</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>freq_pers_predictor_items_cors</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>freq_pers_predictor_items_cors</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>freq_pers_predictor_items_cors</t>
         </is>
@@ -435,42 +405,16 @@
           <t>tends to be quiet.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>bfi1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>tends to be quiet.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>bfi1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>tends to be quiet.</t>
-        </is>
-      </c>
-      <c r="H2">
+      <c r="D2">
         <v>-0.14</v>
       </c>
-      <c r="I2">
+      <c r="E2">
         <v>-0.17</v>
       </c>
-      <c r="J2">
+      <c r="F2">
         <v>0.29</v>
       </c>
-      <c r="K2">
-        <v>0.11</v>
-      </c>
-      <c r="L2">
-        <v>0.11</v>
-      </c>
-      <c r="M2">
+      <c r="G2">
         <v>0.11</v>
       </c>
     </row>
@@ -485,39 +429,13 @@
           <t>When I want to feel less negative emotion (such as sadness or anger), I change what I’m thinking about</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ERQ3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>When I want to feel less negative emotion (such as sadness or anger), I change what I’m thinking about</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ERQ3</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>When I want to feel less negative emotion (such as sadness or anger), I change what I’m thinking about</t>
-        </is>
+      <c r="C3">
+        <v>0.31</v>
+      </c>
+      <c r="F3">
+        <v>0.24</v>
       </c>
       <c r="G3">
-        <v>0.31</v>
-      </c>
-      <c r="J3">
-        <v>0.24</v>
-      </c>
-      <c r="K3">
-        <v>0.11</v>
-      </c>
-      <c r="L3">
-        <v>0.11</v>
-      </c>
-      <c r="M3">
         <v>0.11</v>
       </c>
     </row>
@@ -532,36 +450,10 @@
           <t>When I’m faced with a stressful situation, I make myself think about it in a way that helps me stay calm.</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ERQ5</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>When I’m faced with a stressful situation, I make myself think about it in a way that helps me stay calm.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>ERQ5</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>When I’m faced with a stressful situation, I make myself think about it in a way that helps me stay calm.</t>
-        </is>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0.18</v>
-      </c>
-      <c r="L4">
-        <v>0.18</v>
-      </c>
-      <c r="M4">
         <v>0.18</v>
       </c>
     </row>
@@ -576,39 +468,13 @@
           <t>Like to tidy up.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ipc2_2</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Like to tidy up.</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>ipc2_2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Like to tidy up.</t>
-        </is>
-      </c>
-      <c r="H5">
+      <c r="D5">
         <v>0.11</v>
       </c>
-      <c r="I5">
+      <c r="E5">
         <v>0.4</v>
       </c>
-      <c r="K5">
-        <v>0.1</v>
-      </c>
-      <c r="L5">
-        <v>0.1</v>
-      </c>
-      <c r="M5">
+      <c r="G5">
         <v>0.1</v>
       </c>
     </row>
@@ -623,36 +489,10 @@
           <t>don´t take good care of my belongings*</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ipc2_5</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>don´t take good care of my belongings*</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ipc2_5</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>don´t take good care of my belongings*</t>
-        </is>
-      </c>
-      <c r="I6">
+      <c r="E6">
         <v>0.61</v>
       </c>
-      <c r="K6">
-        <v>-0.12</v>
-      </c>
-      <c r="L6">
-        <v>-0.12</v>
-      </c>
-      <c r="M6">
+      <c r="G6">
         <v>-0.12</v>
       </c>
     </row>
@@ -667,39 +507,13 @@
           <t>Do the opposite of what is asked.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ipc3_6</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Do the opposite of what is asked.</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ipc3_6</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Do the opposite of what is asked.</t>
-        </is>
-      </c>
-      <c r="I7">
+      <c r="E7">
         <v>0.39</v>
       </c>
-      <c r="J7">
+      <c r="F7">
         <v>0.11</v>
       </c>
-      <c r="K7">
-        <v>-0.14</v>
-      </c>
-      <c r="L7">
-        <v>-0.14</v>
-      </c>
-      <c r="M7">
+      <c r="G7">
         <v>-0.14</v>
       </c>
     </row>
@@ -714,39 +528,13 @@
           <t>If there is something I should do, I get to it before attending to lesser tasks.</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ips2</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>If there is something I should do, I get to it before attending to lesser tasks.</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>ips2</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>If there is something I should do, I get to it before attending to lesser tasks.</t>
-        </is>
-      </c>
-      <c r="I8">
+      <c r="E8">
         <v>-0.14</v>
       </c>
-      <c r="J8">
+      <c r="F8">
         <v>-0.26</v>
       </c>
-      <c r="K8">
-        <v>-0.09</v>
-      </c>
-      <c r="L8">
-        <v>-0.09</v>
-      </c>
-      <c r="M8">
+      <c r="G8">
         <v>-0.09</v>
       </c>
     </row>
@@ -761,39 +549,13 @@
           <t>I use different regulatory strategies depending on the situation.</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>MISCS12</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>I use different regulatory strategies depending on the situation.</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>MISCS12</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>I use different regulatory strategies depending on the situation.</t>
-        </is>
-      </c>
-      <c r="H9">
+      <c r="D9">
         <v>0.22</v>
       </c>
-      <c r="J9">
+      <c r="F9">
         <v>0.35</v>
       </c>
-      <c r="K9">
-        <v>0.12</v>
-      </c>
-      <c r="L9">
-        <v>0.12</v>
-      </c>
-      <c r="M9">
+      <c r="G9">
         <v>0.12</v>
       </c>
     </row>
@@ -808,36 +570,10 @@
           <t>I find myself analyzing the usefulness of strategies during self-control conflicts.</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>MISCS19</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>I find myself analyzing the usefulness of strategies during self-control conflicts.</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>MISCS19</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>I find myself analyzing the usefulness of strategies during self-control conflicts.</t>
-        </is>
-      </c>
-      <c r="H10">
+      <c r="D10">
         <v>0.68</v>
       </c>
-      <c r="K10">
-        <v>0.14</v>
-      </c>
-      <c r="L10">
-        <v>0.14</v>
-      </c>
-      <c r="M10">
+      <c r="G10">
         <v>0.14</v>
       </c>
     </row>
@@ -852,36 +588,10 @@
           <t>I find myself pausing regularly to check how well I am resolving a self-control conflict.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>MISCS23</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>I find myself pausing regularly to check how well I am resolving a self-control conflict.</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>MISCS23</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>I find myself pausing regularly to check how well I am resolving a self-control conflict.</t>
-        </is>
-      </c>
-      <c r="H11">
+      <c r="D11">
         <v>0.59</v>
       </c>
-      <c r="K11">
-        <v>0.14</v>
-      </c>
-      <c r="L11">
-        <v>0.14</v>
-      </c>
-      <c r="M11">
+      <c r="G11">
         <v>0.14</v>
       </c>
     </row>
@@ -896,36 +606,10 @@
           <t>I understand my strengths and weaknesses when dealing with self-control conflicts.</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>MISCS4</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>I understand my strengths and weaknesses when dealing with self-control conflicts.</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>MISCS4</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>I understand my strengths and weaknesses when dealing with self-control conflicts.</t>
-        </is>
-      </c>
-      <c r="J12">
+      <c r="F12">
         <v>0.54</v>
       </c>
-      <c r="K12">
-        <v>-0.09</v>
-      </c>
-      <c r="L12">
-        <v>-0.09</v>
-      </c>
-      <c r="M12">
+      <c r="G12">
         <v>-0.09</v>
       </c>
     </row>

</xml_diff>